<commit_message>
wtf shift rows have bug.
</commit_message>
<xml_diff>
--- a/src/main/resources/data/Test.xlsx
+++ b/src/main/resources/data/Test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wei.he1/IdeaProjects/project-world/src/main/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4ADAE8-2B6D-7842-ADCF-BAFB3FFCC2B5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19092A2A-860D-A64F-848D-6CD26DDD213B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2980" yWindow="1900" windowWidth="28240" windowHeight="17440" xr2:uid="{C496940C-3547-8640-A70A-F5CB3E6C52F2}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="1">
   <si>
     <t>Twerwq</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -401,7 +401,7 @@
   <dimension ref="A1:A23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -482,43 +482,43 @@
       </c>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" t="s">
-        <v>0</v>
+      <c r="A16">
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" t="s">
-        <v>0</v>
+      <c r="A17">
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" t="s">
-        <v>0</v>
+      <c r="A18">
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" t="s">
-        <v>0</v>
+      <c r="A19">
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" t="s">
-        <v>0</v>
+      <c r="A20">
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" t="s">
-        <v>0</v>
+      <c r="A21">
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" t="s">
-        <v>0</v>
+      <c r="A22">
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" t="s">
-        <v>0</v>
+      <c r="A23">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>